<commit_message>
first push: created .java folder
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChart.xlsx
+++ b/CS401ProjectGnattChart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F0732A-39B7-1545-A79B-28323DF39E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFFA671-34DA-AE4F-A6A4-DECF04F75369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32840" yWindow="740" windowWidth="32140" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -921,6 +921,13 @@
     <xf numFmtId="0" fontId="23" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -933,13 +940,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1809,8 +1809,8 @@
   <dimension ref="A1:BS49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BM4" sqref="BM4:BS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1823,7 +1823,8 @@
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="2.6640625" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.5" customWidth="1"/>
+    <col min="9" max="70" width="2.5" customWidth="1"/>
+    <col min="71" max="71" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1858,127 +1859,127 @@
         <v>25</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="72">
+      <c r="D3" s="70"/>
+      <c r="E3" s="75">
         <v>43878</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="69">
+      <c r="I4" s="72">
         <f>I5</f>
         <v>43878</v>
       </c>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="69">
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="72">
         <f>P5</f>
         <v>43885</v>
       </c>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="71"/>
-      <c r="W4" s="69">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="72">
         <f>W5</f>
         <v>43892</v>
       </c>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="69">
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="72">
         <f>AD5</f>
         <v>43899</v>
       </c>
-      <c r="AE4" s="70"/>
-      <c r="AF4" s="70"/>
-      <c r="AG4" s="70"/>
-      <c r="AH4" s="70"/>
-      <c r="AI4" s="70"/>
-      <c r="AJ4" s="71"/>
-      <c r="AK4" s="69">
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="72">
         <f>AK5</f>
         <v>43906</v>
       </c>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="70"/>
-      <c r="AN4" s="70"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="71"/>
-      <c r="AR4" s="69">
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="72">
         <f>AR5</f>
         <v>43913</v>
       </c>
-      <c r="AS4" s="70"/>
-      <c r="AT4" s="70"/>
-      <c r="AU4" s="70"/>
-      <c r="AV4" s="70"/>
-      <c r="AW4" s="70"/>
-      <c r="AX4" s="71"/>
-      <c r="AY4" s="69">
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="72">
         <f>AY5</f>
         <v>43920</v>
       </c>
-      <c r="AZ4" s="70"/>
-      <c r="BA4" s="70"/>
-      <c r="BB4" s="70"/>
-      <c r="BC4" s="70"/>
-      <c r="BD4" s="70"/>
-      <c r="BE4" s="71"/>
-      <c r="BF4" s="69">
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="72">
         <f>BF5</f>
         <v>43927</v>
       </c>
-      <c r="BG4" s="70"/>
-      <c r="BH4" s="70"/>
-      <c r="BI4" s="70"/>
-      <c r="BJ4" s="70"/>
-      <c r="BK4" s="70"/>
-      <c r="BL4" s="71"/>
-      <c r="BM4" s="69">
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="74"/>
+      <c r="BM4" s="72">
         <f>BM5</f>
         <v>43934</v>
       </c>
-      <c r="BN4" s="70"/>
-      <c r="BO4" s="70"/>
-      <c r="BP4" s="70"/>
-      <c r="BQ4" s="70"/>
-      <c r="BR4" s="70"/>
-      <c r="BS4" s="71"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="74"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43878</v>
@@ -6064,11 +6065,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -6077,6 +6073,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7">

</xml_diff>